<commit_message>
working on ANU talk
</commit_message>
<xml_diff>
--- a/docs/talks/ANU talk/figs/protein_proportions.xlsx
+++ b/docs/talks/ANU talk/figs/protein_proportions.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\stuff\PEPMOB\D14\docs\talks\ANU talk\figs\"/>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="protein_proportions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>func</t>
   </si>
@@ -64,6 +64,51 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>Calvin cycle</t>
+  </si>
+  <si>
+    <t>light reactions</t>
+  </si>
+  <si>
+    <t>photorespiration</t>
+  </si>
+  <si>
+    <t>protein synthesis</t>
+  </si>
+  <si>
+    <t>stress response</t>
+  </si>
+  <si>
+    <t>37% other</t>
+  </si>
+  <si>
+    <t>63% rubisco</t>
+  </si>
+  <si>
+    <t>photosystems 71</t>
+  </si>
+  <si>
+    <t>ATP synth 22</t>
+  </si>
+  <si>
+    <t>e transport 7</t>
+  </si>
+  <si>
+    <t>ATP synthase (chloroplastic)</t>
+  </si>
+  <si>
+    <t>electron transport</t>
+  </si>
+  <si>
+    <t>photosystems</t>
+  </si>
+  <si>
+    <t>rubisco</t>
+  </si>
+  <si>
+    <t>other Calvin cycle</t>
   </si>
 </sst>
 </file>
@@ -621,19 +666,40 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.22518648805262975"/>
-          <c:y val="8.4560661501065337E-2"/>
-          <c:w val="0.52192139618911271"/>
-          <c:h val="0.74491105499269572"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
@@ -643,263 +709,252 @@
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="10"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
@@ -917,9 +972,737 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>protein_proportions!$A$18:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Calvin cycle</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>light reactions</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>photorespiration</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>protein synthesis</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>stress response</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>protein_proportions!$B$18:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9782.2266659590696</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6489.7311228359704</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>989.08598597437901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2045.7102747122899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>598.95073679043503</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8607.0704541486593</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>protein_proportions!$A$18:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Calvin cycle</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>light reactions</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>photorespiration</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>protein synthesis</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>stress response</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>protein_proportions!$C$18:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.449922460079755</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40377458630482199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42799046433279803</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.418824173939355</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46897803106837299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>CBC</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -959,456 +1742,29 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>protein_proportions!$A$3:$A$13</c:f>
+              <c:f>protein_proportions!$A$29:$A$30</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Calvin_cycle</c:v>
+                  <c:v>rubisco</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Light_reactions</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Photorespiration</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>protein</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>redox</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>stress</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>CHO_metabolism</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>glycolysis</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>RNA</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>TCA_org_transformation</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>other</c:v>
+                  <c:v>other Calvin cycle</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>protein_proportions!$B$3:$B$13</c:f>
+              <c:f>protein_proportions!$B$29:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9782.2266659590696</c:v>
+                  <c:v>6155.7651623440697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6489.7311228359704</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>989.08598597437901</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2045.7102747122899</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>820.24046555070299</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>598.95073679043503</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>519.02223321929603</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>490.95798879892402</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>399.41940146072602</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>345.46308154847299</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6031.9672835705351</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>protein_proportions!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CV_abundance</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="10"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="inEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>protein_proportions!$C$2:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.38049320220757099</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.449922460079755</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.40377458630482199</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.42799046433279803</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.418824173939355</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.39341668072999297</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.46897803106837299</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.40676638088818701</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.405803527983988</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.600858914881093</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.39145491139223598</c:v>
+                  <c:v>3626.4615036149999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1435,17 +1791,395 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="8.6971810341889083E-2"/>
-          <c:y val="0.83309245053794345"/>
-          <c:w val="0.87973603299587555"/>
-          <c:h val="0.1658952384603454"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>LRs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>protein_proportions!$A$31:$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>photosystems</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ATP synthase (chloroplastic)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>electron transport</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>protein_proportions!$B$31:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4574.0942613286097</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1402.99257515515</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>479.33473470180598</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1552,8 +2286,88 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="344">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1576,6 +2390,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
@@ -1583,7 +2408,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1606,9 +2431,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -1640,60 +2468,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:scene3d>
-        <a:camera prst="orthographicFront"/>
-        <a:lightRig rig="brightRoom" dir="t"/>
-      </a:scene3d>
-      <a:sp3d prstMaterial="flat">
-        <a:bevelT w="50800" h="101600" prst="angle"/>
-        <a:contourClr>
-          <a:srgbClr val="000000"/>
-        </a:contourClr>
-      </a:sp3d>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1702,22 +2505,22 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
@@ -1726,8 +2529,8 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1769,23 +2572,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1832,14 +2634,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -1890,8 +2686,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1929,20 +2725,20 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1955,6 +2751,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1986,7 +2793,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" i="0" kern="1200" cap="all" spc="50" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1995,14 +2802,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2023,24 +2829,393 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="344">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2051,20 +3226,648 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="344">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:spPr>
       <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2073,20 +3876,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2101,48 +3904,108 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>328612</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1576387</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>138112</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Marquee">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="5E5E5E"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="DDDDDD"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="418AB3"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="A6B727"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="F69200"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="838383"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="FEC306"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="DF5327"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="F59E00"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="B2B2B2"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -2367,10 +4230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,6 +4383,237 @@
         <v>6031.9672835705351</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>28512.7752404208</v>
+      </c>
+      <c r="C17">
+        <v>0.38049320220757099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>9782.2266659590696</v>
+      </c>
+      <c r="C18">
+        <v>0.449922460079755</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>6489.7311228359704</v>
+      </c>
+      <c r="C19">
+        <v>0.40377458630482199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>989.08598597437901</v>
+      </c>
+      <c r="C20">
+        <v>0.42799046433279803</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>2045.7102747122899</v>
+      </c>
+      <c r="C21">
+        <v>0.418824173939355</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>598.95073679043503</v>
+      </c>
+      <c r="C22">
+        <v>0.46897803106837299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <f>B17 - SUM(B18:B22)</f>
+        <v>8607.0704541486593</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>28512.7752404208</v>
+      </c>
+      <c r="C28">
+        <v>0.38049320220757099</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>6155.7651623440697</v>
+      </c>
+      <c r="C29">
+        <v>0.50103904548479805</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f>9782.22666595907-B29</f>
+        <v>3626.4615036149999</v>
+      </c>
+      <c r="C30">
+        <v>0.449922460079755</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>4574.0942613286097</v>
+      </c>
+      <c r="C31">
+        <v>0.41516379447683399</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <v>1402.99257515515</v>
+      </c>
+      <c r="C32">
+        <v>0.44393386910371002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33">
+        <v>479.33473470180598</v>
+      </c>
+      <c r="C33">
+        <v>0.42449993432368899</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>989.08598597437901</v>
+      </c>
+      <c r="C34">
+        <v>0.42799046433279803</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>2045.7102747122899</v>
+      </c>
+      <c r="C35">
+        <v>0.418824173939355</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <v>598.95073679043503</v>
+      </c>
+      <c r="C36">
+        <v>0.46897803106837299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <f>B28 - SUM(B29:B36)</f>
+        <v>8640.3800057990629</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C19">
     <sortCondition descending="1" ref="B2:B19"/>

</xml_diff>

<commit_message>
split out LHCs into their own categories, added a script with some new plots
</commit_message>
<xml_diff>
--- a/docs/talks/ANU talk/figs/protein_proportions.xlsx
+++ b/docs/talks/ANU talk/figs/protein_proportions.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="protein_proportions" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>func</t>
   </si>
@@ -109,6 +110,24 @@
   </si>
   <si>
     <t>other Calvin cycle</t>
+  </si>
+  <si>
+    <t>bin_arch_name</t>
+  </si>
+  <si>
+    <t>mean_abund</t>
+  </si>
+  <si>
+    <t>CV_abund</t>
+  </si>
+  <si>
+    <t>sd_abund</t>
+  </si>
+  <si>
+    <t>ATP_synthase_chloroplastic</t>
+  </si>
+  <si>
+    <t>light_reactions</t>
   </si>
 </sst>
 </file>
@@ -2246,6 +2265,1009 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>all</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Calvin_cycle</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>light_reactions</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>photorespiration</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>protein</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>stress</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>13454.252039638701</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14823.383996503801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2131.2123837373101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4328.4304914017002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1097.8308833282499</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17689.480170803537</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="78000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="lt1"/>
+      </a:bgClr>
+    </a:pattFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Photosystems</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$14:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>photosystems</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ATP_synthase_chloroplastic</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>electron transport</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8933.7712973407197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4781.4686755071898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1033.99702219695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="78000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="lt1"/>
+      </a:bgClr>
+    </a:pattFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="25000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$21:$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>rubisco</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Calvin cycle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$21:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5474.0561980114198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7980.195841627281</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="78000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="lt1"/>
+      </a:bgClr>
+    </a:pattFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2366,6 +3388,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="344">
   <cs:axisTitle>
@@ -3867,6 +5009,1599 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="261">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="261">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="261">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -3950,6 +6685,101 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>596349</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>124239</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>107674</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28987</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>65431</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>99391</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>49695</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1834598</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>90280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>166480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4232,7 +7062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -4621,4 +7451,237 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>13454.252039638701</v>
+      </c>
+      <c r="C2">
+        <v>0.53575497681506701</v>
+      </c>
+      <c r="D2">
+        <v>7208.1824895607197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>14823.383996503801</v>
+      </c>
+      <c r="C3">
+        <v>0.47733120203868101</v>
+      </c>
+      <c r="D3">
+        <v>7075.6637013320997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>2131.2123837373101</v>
+      </c>
+      <c r="C4">
+        <v>0.50506898792555499</v>
+      </c>
+      <c r="D4">
+        <v>1076.40928170861</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4328.4304914017002</v>
+      </c>
+      <c r="C5">
+        <v>0.48527276799768598</v>
+      </c>
+      <c r="D5">
+        <v>2100.4694456480902</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>1097.8308833282499</v>
+      </c>
+      <c r="C6">
+        <v>0.54088528647977596</v>
+      </c>
+      <c r="D6">
+        <v>593.800571835347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <f>B8-SUM(B2:B6)</f>
+        <v>17689.480170803537</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>53524.589965413303</v>
+      </c>
+      <c r="C8">
+        <v>0.46083148322506901</v>
+      </c>
+      <c r="D8">
+        <v>24665.816182775001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>8933.7712973407197</v>
+      </c>
+      <c r="C14">
+        <v>0.486386325585554</v>
+      </c>
+      <c r="D14">
+        <v>4345.2641949352401</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15">
+        <v>4781.4686755071898</v>
+      </c>
+      <c r="C15">
+        <v>0.53241211388012899</v>
+      </c>
+      <c r="D15">
+        <v>2545.7118449784002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>1033.99702219695</v>
+      </c>
+      <c r="C16">
+        <v>0.48720312483314798</v>
+      </c>
+      <c r="D16">
+        <v>503.76658028252501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>13454.252039638701</v>
+      </c>
+      <c r="C20">
+        <v>0.53575497681506701</v>
+      </c>
+      <c r="D20">
+        <v>7208.1824895607197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>5474.0561980114198</v>
+      </c>
+      <c r="C21">
+        <v>0.63270236485386</v>
+      </c>
+      <c r="D21">
+        <v>3463.4483018247502</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <f>B20-B21</f>
+        <v>7980.195841627281</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>